<commit_message>
added hyphen for post- , and the meaning for H and M in document
</commit_message>
<xml_diff>
--- a/analysis/data/Supplementary_Online_Materials/KWL_layer_assign_details.xlsx
+++ b/analysis/data/Supplementary_Online_Materials/KWL_layer_assign_details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/Supplementary_Information/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA12227B-08DF-1F44-817D-364494AB6828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84447D25-8209-1A42-BEBC-5336537DE646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16540" xr2:uid="{8078604F-F89D-654A-983C-649D14E5F3E8}"/>
   </bookViews>
@@ -350,9 +350,6 @@
     <t>observations on artifacts &amp; features based on field note</t>
   </si>
   <si>
-    <t xml:space="preserve">small jar pieces in L8-L9 (&lt; 20g), likely postdepositional disturbance </t>
-  </si>
-  <si>
     <t>The start of European phase (17th)</t>
   </si>
   <si>
@@ -437,9 +434,6 @@
     <t>increasing charcoals and potsherds beginning from L6, color changes to darker in L8</t>
   </si>
   <si>
-    <t xml:space="preserve">pieces of jar in L5-16, likely postdepositional disturbance </t>
-  </si>
-  <si>
     <t>pieces of jar in L9-L12, likely from middens</t>
   </si>
   <si>
@@ -455,33 +449,21 @@
     <t>European phase indicated by jars in L7 with color change</t>
   </si>
   <si>
-    <t xml:space="preserve">jar pieces in L9 and L10 &lt; 10g, likely postdepositional disturbance </t>
-  </si>
-  <si>
     <t xml:space="preserve">European phase indicated by higher proportion of jars with darker color in L8 </t>
   </si>
   <si>
-    <t>a small piece in L10, likely postdepositional disturbance</t>
-  </si>
-  <si>
     <t xml:space="preserve">European phase indicated by higher proportion of jars with darker color in L9 </t>
   </si>
   <si>
     <t xml:space="preserve">European phase indicated by higher proportion of jars and stoneware with darker color in L9 </t>
   </si>
   <si>
-    <t>jar pieces in L10 &lt; 10g, likely postdepositional disturbance</t>
-  </si>
-  <si>
     <t xml:space="preserve">European phase indicated by higher proportion of jars, and stoneware and pipe in L9 </t>
   </si>
   <si>
     <t>European phase indicated by jars and pipes in L9 with color change</t>
   </si>
   <si>
-    <t>small pieces in L7 &lt; 10g, likely postdepositional disturbance</t>
-  </si>
-  <si>
     <t>European phase indicated by jars and stonewares in L5</t>
   </si>
   <si>
@@ -530,9 +512,6 @@
     <t>European phase indicated by jar in L5 with darker soil color</t>
   </si>
   <si>
-    <t>jar pieces in L6 &lt; 10g, likely postdepositional disturbance. The top of L6 might relate to L5, but it is 20cm thick so excluded</t>
-  </si>
-  <si>
     <t>European phase indicated by jar in L7 with darker soil color</t>
   </si>
   <si>
@@ -563,9 +542,6 @@
     <t>jars in L7 &lt; 30g and L8 &lt; 70g, likely coming from midden</t>
   </si>
   <si>
-    <t xml:space="preserve">jar pieces in L7 &lt; 10g, likely postdepositional disturbance </t>
-  </si>
-  <si>
     <t>European phase indicated by jar in L6 with dark soil color</t>
   </si>
   <si>
@@ -584,9 +560,6 @@
     <t>pieces of jars in L8, liking coming from midden</t>
   </si>
   <si>
-    <t>jar pieces in L8 &lt; 10g, likely postdepositional disturbance, and pieces in L7 might come from midden</t>
-  </si>
-  <si>
     <t>black color in L4-L5 observed on west wall</t>
   </si>
   <si>
@@ -620,21 +593,9 @@
     <t>more local pots in L5</t>
   </si>
   <si>
-    <t>one piece of jar in L6 &gt; 120g, likely postdepositional disturbance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">small jar pieces in L7 &lt; 10g, likely postdepositional disturbance </t>
-  </si>
-  <si>
     <t>H032 = H044, pieces of jar and pipe in L10-L12 might come from middens</t>
   </si>
   <si>
-    <t>small pieces of jar in L10-L13 &lt; 20g, likely postdepositional disturbance</t>
-  </si>
-  <si>
-    <t>small pieces in L9-L12 &lt; 10g, likely postdepositional disturbance</t>
-  </si>
-  <si>
     <t>pieces of jar in L4-L6, likely coming from midden</t>
   </si>
   <si>
@@ -803,9 +764,6 @@
     <t>more artifacts and charcoals in L10-L11</t>
   </si>
   <si>
-    <t xml:space="preserve">C14 dates seem not very reasonable indicating disturbance or contamination of samples. Small pieces of jar in L12, , likely postdepositional disturbance </t>
-  </si>
-  <si>
     <t>European phase indicated by Anping jars and color change in L8 with the reference of radiocarbon date of L7</t>
   </si>
   <si>
@@ -909,6 +867,48 @@
   </si>
   <si>
     <t>European phase indicated by more pieces of Anping jars in L5 with the references of more potsherds and radiocarbon dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small jar pieces in L8-L9 (&lt; 20g), likely post-depositional disturbance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">small jar pieces in L7 &lt; 10g, likely post-depositional disturbance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14 dates seem not very reasonable indicating disturbance or contamination of samples. Small pieces of jar in L12, , likely post-depositional disturbance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pieces of jar in L5-16, likely post-depositional disturbance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jar pieces in L9 and L10 &lt; 10g, likely post-depositional disturbance </t>
+  </si>
+  <si>
+    <t>a small piece in L10, likely post-depositional disturbance</t>
+  </si>
+  <si>
+    <t>jar pieces in L10 &lt; 10g, likely post-depositional disturbance</t>
+  </si>
+  <si>
+    <t>small pieces of jar in L10-L13 &lt; 20g, likely post-depositional disturbance</t>
+  </si>
+  <si>
+    <t>small pieces in L7 &lt; 10g, likely post-depositional disturbance</t>
+  </si>
+  <si>
+    <t>small pieces in L9-L12 &lt; 10g, likely post-depositional disturbance</t>
+  </si>
+  <si>
+    <t>jar pieces in L6 &lt; 10g, likely post-depositional disturbance. The top of L6 might relate to L5, but it is 20cm thick so excluded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jar pieces in L7 &lt; 10g, likely post-depositional disturbance </t>
+  </si>
+  <si>
+    <t>jar pieces in L8 &lt; 10g, likely post-depositional disturbance, and pieces in L7 might come from midden</t>
+  </si>
+  <si>
+    <t>one piece of jar in L6 &gt; 120g, likely post-depositional disturbance</t>
   </si>
 </sst>
 </file>
@@ -1287,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B88541E-9DAB-0E45-BDCD-701CF40445C7}">
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1367,22 +1367,22 @@
         <v>95</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="51" x14ac:dyDescent="0.2">
@@ -1390,7 +1390,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>63</v>
@@ -1408,10 +1408,10 @@
         <v>8</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>105</v>
+        <v>278</v>
       </c>
       <c r="S2" s="2">
         <v>1</v>
@@ -1423,10 +1423,10 @@
         <v>14</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>6</v>
@@ -1461,10 +1461,10 @@
         <v>97</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>196</v>
+        <v>279</v>
       </c>
       <c r="S3" s="2">
         <v>1</v>
@@ -1476,10 +1476,10 @@
         <v>14</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>4</v>
@@ -1509,7 +1509,7 @@
         <v>47</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S4" s="4">
         <v>3</v>
@@ -1521,10 +1521,10 @@
         <v>14</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>0</v>
@@ -1538,7 +1538,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>63</v>
@@ -1556,10 +1556,10 @@
         <v>98</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="S5" s="2">
         <v>1</v>
@@ -1571,10 +1571,10 @@
         <v>14</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>10</v>
@@ -1588,10 +1588,10 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>78</v>
@@ -1609,10 +1609,10 @@
         <v>94</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="S6" s="2">
         <v>1</v>
@@ -1624,10 +1624,10 @@
         <v>14</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>7</v>
@@ -1668,10 +1668,10 @@
         <v>11</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S7" s="2">
         <v>1</v>
@@ -1683,10 +1683,10 @@
         <v>14</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>7</v>
@@ -1718,10 +1718,10 @@
         <v>5</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>134</v>
+        <v>281</v>
       </c>
       <c r="S8" s="2">
         <v>2</v>
@@ -1733,10 +1733,10 @@
         <v>14</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>3</v>
@@ -1762,25 +1762,25 @@
         <v>5</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S9" s="2">
         <v>1</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>5</v>
@@ -1794,7 +1794,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>63</v>
@@ -1809,7 +1809,7 @@
         <v>6</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>23</v>
@@ -1818,16 +1818,16 @@
         <v>1</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>6</v>
@@ -1841,10 +1841,10 @@
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>77</v>
@@ -1871,22 +1871,22 @@
         <v>25</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>140</v>
+        <v>282</v>
       </c>
       <c r="S11" s="2">
         <v>1</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="X11" s="2" t="s">
         <v>7</v>
@@ -1900,16 +1900,16 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>64</v>
@@ -1933,25 +1933,25 @@
         <v>9</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>142</v>
+        <v>283</v>
       </c>
       <c r="S12" s="2">
         <v>1</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>8</v>
@@ -1965,16 +1965,16 @@
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>71</v>
@@ -1995,25 +1995,25 @@
         <v>9</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>145</v>
+        <v>284</v>
       </c>
       <c r="S13" s="2">
         <v>1</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="X13" s="2" t="s">
         <v>8</v>
@@ -2027,13 +2027,13 @@
         <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>68</v>
@@ -2060,25 +2060,25 @@
         <v>99</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="S14" s="2">
         <v>1</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>8</v>
@@ -2092,10 +2092,10 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>68</v>
@@ -2122,25 +2122,25 @@
         <v>12</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>198</v>
+        <v>285</v>
       </c>
       <c r="S15" s="2">
         <v>1</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>8</v>
@@ -2154,19 +2154,19 @@
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>64</v>
@@ -2178,7 +2178,7 @@
         <v>41</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>148</v>
+        <v>286</v>
       </c>
       <c r="S16" s="2">
         <v>1</v>
@@ -2190,10 +2190,10 @@
         <v>2</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>4</v>
@@ -2207,22 +2207,22 @@
         <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>64</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>75</v>
@@ -2243,25 +2243,25 @@
         <v>100</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
       <c r="S17" s="2">
         <v>1</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>6</v>
@@ -2275,10 +2275,10 @@
         <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>63</v>
@@ -2287,7 +2287,7 @@
         <v>4</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>33</v>
@@ -2296,16 +2296,16 @@
         <v>1</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>3</v>
@@ -2319,7 +2319,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>64</v>
@@ -2331,10 +2331,10 @@
         <v>102</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="S19" s="2">
         <v>1</v>
@@ -2346,10 +2346,10 @@
         <v>0</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>2</v>
@@ -2363,7 +2363,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>64</v>
@@ -2387,25 +2387,25 @@
         <v>9</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="S20" s="2">
         <v>1</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="X20" s="2" t="s">
         <v>5</v>
@@ -2419,22 +2419,22 @@
         <v>36</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>65</v>
@@ -2449,7 +2449,7 @@
         <v>9</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>91</v>
@@ -2458,16 +2458,16 @@
         <v>1</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="X21" s="2" t="s">
         <v>9</v>
@@ -2481,19 +2481,19 @@
         <v>37</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>72</v>
@@ -2514,10 +2514,10 @@
         <v>12</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="S22" s="2">
         <v>1</v>
@@ -2526,13 +2526,13 @@
         <v>9</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="X22" s="2" t="s">
         <v>10</v>
@@ -2546,19 +2546,19 @@
         <v>38</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>63</v>
@@ -2585,25 +2585,25 @@
         <v>11</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="S23" s="2">
         <v>1</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="X23" s="2" t="s">
         <v>8</v>
@@ -2617,13 +2617,13 @@
         <v>39</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>64</v>
@@ -2632,25 +2632,25 @@
         <v>7</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="S24" s="2">
         <v>1</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="X24" s="2" t="s">
         <v>7</v>
@@ -2664,19 +2664,19 @@
         <v>40</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>64</v>
@@ -2691,25 +2691,25 @@
         <v>10</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="S25" s="2">
         <v>1</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="X25" s="2" t="s">
         <v>5</v>
@@ -2723,16 +2723,16 @@
         <v>42</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>64</v>
@@ -2744,10 +2744,10 @@
         <v>5</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>165</v>
+        <v>288</v>
       </c>
       <c r="S26" s="2">
         <v>1</v>
@@ -2756,13 +2756,13 @@
         <v>4</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="X26" s="2" t="s">
         <v>4</v>
@@ -2776,16 +2776,16 @@
         <v>43</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>64</v>
@@ -2806,13 +2806,13 @@
         <v>6</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="X27" s="2" t="s">
         <v>6</v>
@@ -2826,13 +2826,13 @@
         <v>44</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>64</v>
@@ -2844,7 +2844,7 @@
         <v>6</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>23</v>
@@ -2853,16 +2853,16 @@
         <v>1</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="X28" s="2" t="s">
         <v>6</v>
@@ -2876,13 +2876,13 @@
         <v>45</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>67</v>
@@ -2894,7 +2894,7 @@
         <v>4</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>92</v>
@@ -2903,16 +2903,16 @@
         <v>1</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="X29" s="2" t="s">
         <v>4</v>
@@ -2926,17 +2926,17 @@
         <v>46</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>93</v>
@@ -2951,10 +2951,10 @@
         <v>14</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="X30" s="4" t="s">
         <v>1</v>
@@ -2968,10 +2968,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>63</v>
@@ -2989,7 +2989,7 @@
         <v>49</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="S31" s="2">
         <v>1</v>
@@ -3001,10 +3001,10 @@
         <v>14</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="X31" s="2" t="s">
         <v>3</v>
@@ -3018,7 +3018,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>64</v>
@@ -3042,7 +3042,7 @@
         <v>51</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="S32" s="2">
         <v>1</v>
@@ -3054,10 +3054,10 @@
         <v>14</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="X32" s="2" t="s">
         <v>2</v>
@@ -3071,19 +3071,19 @@
         <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="S33" s="2">
         <v>2</v>
@@ -3095,10 +3095,10 @@
         <v>0</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="X33" s="2" t="s">
         <v>1</v>
@@ -3112,10 +3112,10 @@
         <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>63</v>
@@ -3127,10 +3127,10 @@
         <v>3</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="S34" s="2">
         <v>2</v>
@@ -3142,10 +3142,10 @@
         <v>0</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="X34" s="2" t="s">
         <v>1</v>
@@ -3159,16 +3159,16 @@
         <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>83</v>
@@ -3183,25 +3183,25 @@
         <v>7</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="S35" s="2">
         <v>1</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="X35" s="2" t="s">
         <v>4</v>
@@ -3215,10 +3215,10 @@
         <v>55</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>64</v>
@@ -3236,10 +3236,10 @@
         <v>6</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>176</v>
+        <v>289</v>
       </c>
       <c r="S36" s="2">
         <v>1</v>
@@ -3248,13 +3248,13 @@
         <v>5</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="X36" s="2" t="s">
         <v>5</v>
@@ -3268,13 +3268,13 @@
         <v>56</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>64</v>
@@ -3295,25 +3295,25 @@
         <v>9</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="S37" s="2">
         <v>1</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="X37" s="2" t="s">
         <v>7</v>
@@ -3327,13 +3327,13 @@
         <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>68</v>
@@ -3360,10 +3360,10 @@
         <v>101</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="S38" s="2">
         <v>1</v>
@@ -3372,13 +3372,13 @@
         <v>7</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="X38" s="2" t="s">
         <v>8</v>
@@ -3392,16 +3392,16 @@
         <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>70</v>
@@ -3419,25 +3419,25 @@
         <v>8</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="S39" s="2">
         <v>1</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="X39" s="2" t="s">
         <v>6</v>
@@ -3451,16 +3451,16 @@
         <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>64</v>
@@ -3475,25 +3475,25 @@
         <v>7</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>183</v>
+        <v>290</v>
       </c>
       <c r="S40" s="2">
         <v>1</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U40" s="1" t="s">
         <v>1</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="X40" s="2" t="s">
         <v>5</v>
@@ -3507,10 +3507,10 @@
         <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>64</v>
@@ -3528,25 +3528,25 @@
         <v>9</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>145</v>
+        <v>284</v>
       </c>
       <c r="S41" s="2">
         <v>1</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="X41" s="2" t="s">
         <v>6</v>
@@ -3560,10 +3560,10 @@
         <v>61</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>63</v>
@@ -3572,10 +3572,10 @@
         <v>7</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>195</v>
+        <v>291</v>
       </c>
       <c r="S42" s="2">
         <v>2</v>
@@ -3587,10 +3587,10 @@
         <v>14</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="X42" s="2" t="s">
         <v>4</v>

</xml_diff>